<commit_message>
More product Spreadsheets added, new product image.
More product spreadsheets have been added, now there are only a few product spreadsheets that are still missing. Changed the image importing recursive from false to true, this means that it will now look inside of folders.
</commit_message>
<xml_diff>
--- a/models/products.xlsx
+++ b/models/products.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\jakee\Documents\GitHub\thorsmex_digital_catalog\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{85B35303-1952-494A-8EB0-FFECDE4CE32E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1FDB6A2-C6FB-4562-BB7F-A07B8336DFE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="products" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1683" uniqueCount="545">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1683" uniqueCount="552">
   <si>
     <t>model_number</t>
   </si>
@@ -2232,11 +2232,32 @@
   <si>
     <t xml:space="preserve">Wiremold Overfloor Cord Protector (15 Pack) White Final Lid </t>
   </si>
+  <si>
+    <t>CABLE CLIP NAIL IN TC3X5-6X10.pdf</t>
+  </si>
+  <si>
+    <t>SPIRAL CABLE WRAP (ALL VARIATIONS).pdf</t>
+  </si>
+  <si>
+    <t>Canal TMK 0812 EN.pdf</t>
+  </si>
+  <si>
+    <t>Canal TMK 1020 EN.pdf</t>
+  </si>
+  <si>
+    <t>Canal TMK 1720 EN.pdf</t>
+  </si>
+  <si>
+    <t>Canal TMK 1735 EN.pdf</t>
+  </si>
+  <si>
+    <t>SOFT OVERFLOOR CORD PROTECTOR.pdf</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3074,16 +3095,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
-      <selection activeCell="B90" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="I160" sqref="I160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
     <col min="2" max="2" width="14.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -9374,7 +9397,7 @@
         <v>223</v>
       </c>
       <c r="I63" t="s">
-        <v>118</v>
+        <v>545</v>
       </c>
       <c r="J63">
         <v>10.23</v>
@@ -9475,7 +9498,7 @@
         <v>223</v>
       </c>
       <c r="I64" t="s">
-        <v>118</v>
+        <v>545</v>
       </c>
       <c r="J64">
         <v>5.0999999999999996</v>
@@ -9576,7 +9599,7 @@
         <v>259</v>
       </c>
       <c r="I65" t="s">
-        <v>118</v>
+        <v>545</v>
       </c>
       <c r="J65">
         <v>5.0199999999999996</v>
@@ -9677,7 +9700,7 @@
         <v>263</v>
       </c>
       <c r="I66" t="s">
-        <v>118</v>
+        <v>545</v>
       </c>
       <c r="J66">
         <v>8.3699999999999992</v>
@@ -9778,7 +9801,7 @@
         <v>259</v>
       </c>
       <c r="I67" t="s">
-        <v>118</v>
+        <v>545</v>
       </c>
       <c r="J67">
         <v>5.0999999999999996</v>
@@ -9879,7 +9902,7 @@
         <v>270</v>
       </c>
       <c r="I68" t="s">
-        <v>118</v>
+        <v>545</v>
       </c>
       <c r="J68">
         <v>11.52</v>
@@ -9980,7 +10003,7 @@
         <v>270</v>
       </c>
       <c r="I69" t="s">
-        <v>118</v>
+        <v>545</v>
       </c>
       <c r="J69">
         <v>5.44</v>
@@ -10081,7 +10104,7 @@
         <v>270</v>
       </c>
       <c r="I70" t="s">
-        <v>118</v>
+        <v>545</v>
       </c>
       <c r="J70">
         <v>3.22</v>
@@ -10182,7 +10205,7 @@
         <v>279</v>
       </c>
       <c r="I71" t="s">
-        <v>118</v>
+        <v>545</v>
       </c>
       <c r="J71">
         <v>11.52</v>
@@ -10283,7 +10306,7 @@
         <v>279</v>
       </c>
       <c r="I72" t="s">
-        <v>118</v>
+        <v>545</v>
       </c>
       <c r="J72">
         <v>6.78</v>
@@ -10384,7 +10407,7 @@
         <v>286</v>
       </c>
       <c r="I73" t="s">
-        <v>118</v>
+        <v>202</v>
       </c>
       <c r="J73">
         <v>3.1</v>
@@ -10485,7 +10508,7 @@
         <v>286</v>
       </c>
       <c r="I74" t="s">
-        <v>118</v>
+        <v>202</v>
       </c>
       <c r="J74">
         <v>15.86</v>
@@ -10990,7 +11013,7 @@
         <v>314</v>
       </c>
       <c r="I79" t="s">
-        <v>118</v>
+        <v>546</v>
       </c>
       <c r="J79">
         <v>4.13</v>
@@ -11091,7 +11114,7 @@
         <v>319</v>
       </c>
       <c r="I80" t="s">
-        <v>118</v>
+        <v>546</v>
       </c>
       <c r="J80">
         <v>23.71</v>
@@ -11192,7 +11215,7 @@
         <v>324</v>
       </c>
       <c r="I81" t="s">
-        <v>118</v>
+        <v>546</v>
       </c>
       <c r="J81">
         <v>124.67</v>
@@ -11293,7 +11316,7 @@
         <v>314</v>
       </c>
       <c r="I82" t="s">
-        <v>118</v>
+        <v>546</v>
       </c>
       <c r="J82">
         <v>3.37</v>
@@ -11394,7 +11417,7 @@
         <v>309</v>
       </c>
       <c r="I83" t="s">
-        <v>118</v>
+        <v>546</v>
       </c>
       <c r="J83">
         <v>3.37</v>
@@ -11495,7 +11518,7 @@
         <v>314</v>
       </c>
       <c r="I84" t="s">
-        <v>118</v>
+        <v>546</v>
       </c>
       <c r="J84">
         <v>4.13</v>
@@ -11596,7 +11619,7 @@
         <v>319</v>
       </c>
       <c r="I85" t="s">
-        <v>118</v>
+        <v>546</v>
       </c>
       <c r="J85">
         <v>4.13</v>
@@ -11697,7 +11720,7 @@
         <v>324</v>
       </c>
       <c r="I86" t="s">
-        <v>118</v>
+        <v>546</v>
       </c>
       <c r="J86">
         <v>23.71</v>
@@ -11798,7 +11821,7 @@
         <v>309</v>
       </c>
       <c r="I87" t="s">
-        <v>118</v>
+        <v>546</v>
       </c>
       <c r="J87">
         <v>36.81</v>
@@ -11899,7 +11922,7 @@
         <v>314</v>
       </c>
       <c r="I88" t="s">
-        <v>118</v>
+        <v>546</v>
       </c>
       <c r="J88">
         <v>4.12</v>
@@ -12000,7 +12023,7 @@
         <v>319</v>
       </c>
       <c r="I89" t="s">
-        <v>118</v>
+        <v>546</v>
       </c>
       <c r="J89">
         <v>4.13</v>
@@ -12101,7 +12124,7 @@
         <v>324</v>
       </c>
       <c r="I90" t="s">
-        <v>118</v>
+        <v>546</v>
       </c>
       <c r="J90">
         <v>23.71</v>
@@ -12202,7 +12225,7 @@
         <v>314</v>
       </c>
       <c r="I91" t="s">
-        <v>118</v>
+        <v>546</v>
       </c>
       <c r="J91">
         <v>3.06</v>
@@ -12303,7 +12326,7 @@
         <v>309</v>
       </c>
       <c r="I92" t="s">
-        <v>118</v>
+        <v>546</v>
       </c>
       <c r="J92">
         <v>3.37</v>
@@ -12404,7 +12427,7 @@
         <v>314</v>
       </c>
       <c r="I93" t="s">
-        <v>118</v>
+        <v>546</v>
       </c>
       <c r="J93">
         <v>4.12</v>
@@ -12505,7 +12528,7 @@
         <v>319</v>
       </c>
       <c r="I94" t="s">
-        <v>118</v>
+        <v>546</v>
       </c>
       <c r="J94">
         <v>4.13</v>
@@ -12606,7 +12629,7 @@
         <v>324</v>
       </c>
       <c r="I95" t="s">
-        <v>118</v>
+        <v>546</v>
       </c>
       <c r="J95">
         <v>23.71</v>
@@ -12707,7 +12730,7 @@
         <v>309</v>
       </c>
       <c r="I96" t="s">
-        <v>118</v>
+        <v>546</v>
       </c>
       <c r="J96">
         <v>3.37</v>
@@ -12808,7 +12831,7 @@
         <v>358</v>
       </c>
       <c r="I97" t="s">
-        <v>118</v>
+        <v>546</v>
       </c>
       <c r="J97">
         <v>4.12</v>
@@ -12909,7 +12932,7 @@
         <v>319</v>
       </c>
       <c r="I98" t="s">
-        <v>118</v>
+        <v>546</v>
       </c>
       <c r="J98">
         <v>4.13</v>
@@ -13010,7 +13033,7 @@
         <v>324</v>
       </c>
       <c r="I99" t="s">
-        <v>118</v>
+        <v>546</v>
       </c>
       <c r="J99">
         <v>23.71</v>
@@ -13212,7 +13235,7 @@
         <v>368</v>
       </c>
       <c r="I101" t="s">
-        <v>118</v>
+        <v>547</v>
       </c>
       <c r="J101">
         <v>3.87</v>
@@ -13313,7 +13336,7 @@
         <v>368</v>
       </c>
       <c r="I102" t="s">
-        <v>118</v>
+        <v>547</v>
       </c>
       <c r="J102">
         <v>10.76</v>
@@ -13414,7 +13437,7 @@
         <v>368</v>
       </c>
       <c r="I103" t="s">
-        <v>118</v>
+        <v>547</v>
       </c>
       <c r="J103">
         <v>7.08</v>
@@ -13515,7 +13538,7 @@
         <v>368</v>
       </c>
       <c r="I104" t="s">
-        <v>118</v>
+        <v>547</v>
       </c>
       <c r="J104">
         <v>6.82</v>
@@ -13616,7 +13639,7 @@
         <v>380</v>
       </c>
       <c r="I105" t="s">
-        <v>118</v>
+        <v>547</v>
       </c>
       <c r="J105">
         <v>0.77</v>
@@ -13717,7 +13740,7 @@
         <v>380</v>
       </c>
       <c r="I106" t="s">
-        <v>118</v>
+        <v>547</v>
       </c>
       <c r="J106">
         <v>0.77</v>
@@ -13818,7 +13841,7 @@
         <v>380</v>
       </c>
       <c r="I107" t="s">
-        <v>118</v>
+        <v>547</v>
       </c>
       <c r="J107">
         <v>0.77</v>
@@ -13919,7 +13942,7 @@
         <v>380</v>
       </c>
       <c r="I108" t="s">
-        <v>118</v>
+        <v>547</v>
       </c>
       <c r="J108">
         <v>0.77</v>
@@ -14020,7 +14043,7 @@
         <v>380</v>
       </c>
       <c r="I109" t="s">
-        <v>118</v>
+        <v>547</v>
       </c>
       <c r="J109">
         <v>0.81</v>
@@ -14121,7 +14144,7 @@
         <v>380</v>
       </c>
       <c r="I110" t="s">
-        <v>118</v>
+        <v>547</v>
       </c>
       <c r="J110">
         <v>0.81</v>
@@ -14222,7 +14245,7 @@
         <v>398</v>
       </c>
       <c r="I111" t="s">
-        <v>118</v>
+        <v>547</v>
       </c>
       <c r="J111">
         <v>2.92</v>
@@ -14323,7 +14346,7 @@
         <v>402</v>
       </c>
       <c r="I112" t="s">
-        <v>118</v>
+        <v>548</v>
       </c>
       <c r="J112">
         <v>9.7100000000000009</v>
@@ -14424,7 +14447,7 @@
         <v>406</v>
       </c>
       <c r="I113" t="s">
-        <v>118</v>
+        <v>548</v>
       </c>
       <c r="J113">
         <v>11.83</v>
@@ -14525,7 +14548,7 @@
         <v>406</v>
       </c>
       <c r="I114" t="s">
-        <v>118</v>
+        <v>548</v>
       </c>
       <c r="J114">
         <v>11.93</v>
@@ -14626,7 +14649,7 @@
         <v>402</v>
       </c>
       <c r="I115" t="s">
-        <v>118</v>
+        <v>548</v>
       </c>
       <c r="J115">
         <v>11.88</v>
@@ -14727,7 +14750,7 @@
         <v>413</v>
       </c>
       <c r="I116" t="s">
-        <v>118</v>
+        <v>548</v>
       </c>
       <c r="J116">
         <v>17.75</v>
@@ -14828,7 +14851,7 @@
         <v>416</v>
       </c>
       <c r="I117" t="s">
-        <v>118</v>
+        <v>548</v>
       </c>
       <c r="J117">
         <v>12.68</v>
@@ -14929,7 +14952,7 @@
         <v>419</v>
       </c>
       <c r="I118" t="s">
-        <v>118</v>
+        <v>548</v>
       </c>
       <c r="J118">
         <v>12.52</v>
@@ -15030,7 +15053,7 @@
         <v>419</v>
       </c>
       <c r="I119" t="s">
-        <v>118</v>
+        <v>548</v>
       </c>
       <c r="J119">
         <v>12.34</v>
@@ -15131,7 +15154,7 @@
         <v>425</v>
       </c>
       <c r="I120" t="s">
-        <v>118</v>
+        <v>548</v>
       </c>
       <c r="J120">
         <v>7.8</v>
@@ -15232,7 +15255,7 @@
         <v>425</v>
       </c>
       <c r="I121" t="s">
-        <v>118</v>
+        <v>548</v>
       </c>
       <c r="J121">
         <v>8.83</v>
@@ -15333,7 +15356,7 @@
         <v>431</v>
       </c>
       <c r="I122" t="s">
-        <v>118</v>
+        <v>548</v>
       </c>
       <c r="J122">
         <v>13.99</v>
@@ -15434,7 +15457,7 @@
         <v>431</v>
       </c>
       <c r="I123" t="s">
-        <v>118</v>
+        <v>548</v>
       </c>
       <c r="J123">
         <v>12.28</v>
@@ -15535,7 +15558,7 @@
         <v>431</v>
       </c>
       <c r="I124" t="s">
-        <v>118</v>
+        <v>548</v>
       </c>
       <c r="J124">
         <v>9.5399999999999991</v>
@@ -15636,7 +15659,7 @@
         <v>431</v>
       </c>
       <c r="I125" t="s">
-        <v>118</v>
+        <v>548</v>
       </c>
       <c r="J125">
         <v>8.08</v>
@@ -15737,7 +15760,7 @@
         <v>441</v>
       </c>
       <c r="I126" t="s">
-        <v>118</v>
+        <v>549</v>
       </c>
       <c r="J126">
         <v>14.4</v>
@@ -15838,7 +15861,7 @@
         <v>441</v>
       </c>
       <c r="I127" t="s">
-        <v>118</v>
+        <v>549</v>
       </c>
       <c r="J127">
         <v>14.4</v>
@@ -15939,7 +15962,7 @@
         <v>441</v>
       </c>
       <c r="I128" t="s">
-        <v>118</v>
+        <v>549</v>
       </c>
       <c r="J128">
         <v>17.75</v>
@@ -16040,7 +16063,7 @@
         <v>441</v>
       </c>
       <c r="I129" t="s">
-        <v>118</v>
+        <v>549</v>
       </c>
       <c r="J129">
         <v>15.68</v>
@@ -16141,7 +16164,7 @@
         <v>451</v>
       </c>
       <c r="I130" t="s">
-        <v>118</v>
+        <v>549</v>
       </c>
       <c r="J130">
         <v>9.34</v>
@@ -16242,7 +16265,7 @@
         <v>451</v>
       </c>
       <c r="I131" t="s">
-        <v>118</v>
+        <v>549</v>
       </c>
       <c r="J131">
         <v>8.83</v>
@@ -16343,7 +16366,7 @@
         <v>451</v>
       </c>
       <c r="I132" t="s">
-        <v>118</v>
+        <v>549</v>
       </c>
       <c r="J132">
         <v>13.99</v>
@@ -16444,7 +16467,7 @@
         <v>451</v>
       </c>
       <c r="I133" t="s">
-        <v>118</v>
+        <v>549</v>
       </c>
       <c r="J133">
         <v>1.51</v>
@@ -16545,7 +16568,7 @@
         <v>451</v>
       </c>
       <c r="I134" t="s">
-        <v>118</v>
+        <v>549</v>
       </c>
       <c r="J134">
         <v>1.7</v>
@@ -16646,7 +16669,7 @@
         <v>451</v>
       </c>
       <c r="I135" t="s">
-        <v>118</v>
+        <v>549</v>
       </c>
       <c r="J135">
         <v>1.69</v>
@@ -16747,7 +16770,7 @@
         <v>465</v>
       </c>
       <c r="I136" t="s">
-        <v>118</v>
+        <v>550</v>
       </c>
       <c r="J136">
         <v>22.87</v>
@@ -16848,7 +16871,7 @@
         <v>465</v>
       </c>
       <c r="I137" t="s">
-        <v>118</v>
+        <v>550</v>
       </c>
       <c r="J137">
         <v>22.87</v>
@@ -16949,7 +16972,7 @@
         <v>465</v>
       </c>
       <c r="I138" t="s">
-        <v>118</v>
+        <v>550</v>
       </c>
       <c r="J138">
         <v>22.87</v>
@@ -17050,7 +17073,7 @@
         <v>465</v>
       </c>
       <c r="I139" t="s">
-        <v>118</v>
+        <v>550</v>
       </c>
       <c r="J139">
         <v>22.87</v>
@@ -17151,7 +17174,7 @@
         <v>465</v>
       </c>
       <c r="I140" t="s">
-        <v>118</v>
+        <v>550</v>
       </c>
       <c r="J140">
         <v>26.9</v>
@@ -17252,7 +17275,7 @@
         <v>465</v>
       </c>
       <c r="I141" t="s">
-        <v>118</v>
+        <v>550</v>
       </c>
       <c r="J141">
         <v>26.9</v>
@@ -17353,7 +17376,7 @@
         <v>479</v>
       </c>
       <c r="I142" t="s">
-        <v>118</v>
+        <v>550</v>
       </c>
       <c r="J142">
         <v>1.76</v>
@@ -17454,7 +17477,7 @@
         <v>479</v>
       </c>
       <c r="I143" t="s">
-        <v>118</v>
+        <v>550</v>
       </c>
       <c r="J143">
         <v>1.72</v>
@@ -17555,7 +17578,7 @@
         <v>479</v>
       </c>
       <c r="I144" t="s">
-        <v>118</v>
+        <v>550</v>
       </c>
       <c r="J144">
         <v>1.72</v>
@@ -17656,7 +17679,7 @@
         <v>479</v>
       </c>
       <c r="I145" t="s">
-        <v>118</v>
+        <v>550</v>
       </c>
       <c r="J145">
         <v>1.72</v>
@@ -17757,7 +17780,7 @@
         <v>479</v>
       </c>
       <c r="I146" t="s">
-        <v>118</v>
+        <v>550</v>
       </c>
       <c r="J146">
         <v>1.73</v>
@@ -18969,7 +18992,7 @@
         <v>526</v>
       </c>
       <c r="I158" t="s">
-        <v>118</v>
+        <v>551</v>
       </c>
       <c r="J158">
         <v>26.43</v>
@@ -19070,7 +19093,7 @@
         <v>526</v>
       </c>
       <c r="I159" t="s">
-        <v>118</v>
+        <v>551</v>
       </c>
       <c r="J159">
         <v>26.43</v>
@@ -19171,7 +19194,7 @@
         <v>526</v>
       </c>
       <c r="I160" t="s">
-        <v>118</v>
+        <v>551</v>
       </c>
       <c r="J160">
         <v>26.43</v>

</xml_diff>

<commit_message>
Individual counts updated in product spreadsheet
</commit_message>
<xml_diff>
--- a/models/products.xlsx
+++ b/models/products.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\jakee\Documents\GitHub\thorsmex_digital_catalog\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1FDB6A2-C6FB-4562-BB7F-A07B8336DFE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4B7A790-547F-492F-A1D1-313B75D25697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="products" sheetId="1" r:id="rId1"/>
@@ -3098,8 +3098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="I160" sqref="I160"/>
+    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="C163" sqref="C163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3444,7 +3444,7 @@
         <v>5.47</v>
       </c>
       <c r="K4">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="L4">
         <v>492.3</v>
@@ -3646,7 +3646,7 @@
         <v>4.9800000000000004</v>
       </c>
       <c r="K6">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="L6">
         <v>687.24</v>
@@ -3747,7 +3747,7 @@
         <v>4.6900000000000004</v>
       </c>
       <c r="K7">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="L7">
         <v>422.1</v>
@@ -3949,7 +3949,7 @@
         <v>5.29</v>
       </c>
       <c r="K9">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="L9">
         <v>264.5</v>
@@ -4050,7 +4050,7 @@
         <v>2.5299999999999998</v>
       </c>
       <c r="K10">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="L10">
         <v>227.7</v>
@@ -4151,7 +4151,7 @@
         <v>5.41</v>
       </c>
       <c r="K11">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="L11">
         <v>270.5</v>
@@ -4252,7 +4252,7 @@
         <v>13.06</v>
       </c>
       <c r="K12">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="L12">
         <v>992.56</v>
@@ -4454,7 +4454,7 @@
         <v>5.51</v>
       </c>
       <c r="K14">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="L14">
         <v>275.5</v>
@@ -4555,7 +4555,7 @@
         <v>4.5599999999999996</v>
       </c>
       <c r="K15">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="L15">
         <v>410.4</v>
@@ -4757,7 +4757,7 @@
         <v>13.96</v>
       </c>
       <c r="K17">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="L17">
         <v>1005.12</v>
@@ -4858,7 +4858,7 @@
         <v>15.39</v>
       </c>
       <c r="K18">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="L18">
         <v>230.85</v>
@@ -5161,7 +5161,7 @@
         <v>5.86</v>
       </c>
       <c r="K21">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="L21">
         <v>87.9</v>
@@ -5262,7 +5262,7 @@
         <v>12.96</v>
       </c>
       <c r="K22">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="L22">
         <v>1788.48</v>
@@ -5363,7 +5363,7 @@
         <v>10.62</v>
       </c>
       <c r="K23">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="L23">
         <v>573.48</v>
@@ -8898,7 +8898,7 @@
         <v>5.15</v>
       </c>
       <c r="K58">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="L58">
         <v>200.85</v>
@@ -13746,7 +13746,7 @@
         <v>0.77</v>
       </c>
       <c r="K106">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="L106">
         <v>7.7</v>
@@ -16170,7 +16170,7 @@
         <v>9.34</v>
       </c>
       <c r="K130">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="L130">
         <v>93.4</v>

</xml_diff>

<commit_message>
More updates to master file
</commit_message>
<xml_diff>
--- a/models/products.xlsx
+++ b/models/products.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\jakee\Documents\GitHub\thorsmex_digital_catalog\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CBF0303-63F6-4C1B-A9B1-C5F1CD6B134E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{695A1911-EC5B-4B06-B7D0-651A1F7BA961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1683" uniqueCount="514">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1683" uniqueCount="513">
   <si>
     <t>model_number</t>
   </si>
@@ -2015,9 +2015,6 @@
   </si>
   <si>
     <t>Raceway 3.6' (10 Pack)</t>
-  </si>
-  <si>
-    <t>Raceway 3.6' with Adhesive</t>
   </si>
   <si>
     <t>Raceway Transparent Lid 8.2' (25 Pack)</t>
@@ -2984,8 +2981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG166"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C161" sqref="C161"/>
+    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="C122" sqref="C122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -14416,7 +14413,7 @@
         <v>7501509900196</v>
       </c>
       <c r="C114" t="s">
-        <v>473</v>
+        <v>489</v>
       </c>
       <c r="D114" t="s">
         <v>97</v>
@@ -14719,7 +14716,7 @@
         <v>7506218111673</v>
       </c>
       <c r="C117" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D117" t="s">
         <v>97</v>
@@ -14820,7 +14817,7 @@
         <v>7501509900141</v>
       </c>
       <c r="C118" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D118" t="s">
         <v>97</v>
@@ -14921,7 +14918,7 @@
         <v>7501509900165</v>
       </c>
       <c r="C119" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D119" t="s">
         <v>97</v>
@@ -15022,7 +15019,7 @@
         <v>7501509900974</v>
       </c>
       <c r="C120" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D120" t="s">
         <v>97</v>
@@ -15123,7 +15120,7 @@
         <v>7501509900967</v>
       </c>
       <c r="C121" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D121" t="s">
         <v>97</v>
@@ -15224,7 +15221,7 @@
         <v>7501509900981</v>
       </c>
       <c r="C122" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D122" t="s">
         <v>97</v>
@@ -15325,7 +15322,7 @@
         <v>7501509905245</v>
       </c>
       <c r="C123" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D123" t="s">
         <v>97</v>
@@ -15426,7 +15423,7 @@
         <v>7501509905221</v>
       </c>
       <c r="C124" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D124" t="s">
         <v>97</v>
@@ -15527,7 +15524,7 @@
         <v>7501509900998</v>
       </c>
       <c r="C125" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="D125" t="s">
         <v>97</v>
@@ -15628,7 +15625,7 @@
         <v>7501509901001</v>
       </c>
       <c r="C126" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="D126" t="s">
         <v>97</v>
@@ -15830,7 +15827,7 @@
         <v>7501509900202</v>
       </c>
       <c r="C128" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D128" t="s">
         <v>97</v>
@@ -15931,7 +15928,7 @@
         <v>7501509900189</v>
       </c>
       <c r="C129" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D129" t="s">
         <v>97</v>
@@ -16032,7 +16029,7 @@
         <v>7501509901025</v>
       </c>
       <c r="C130" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D130" t="s">
         <v>97</v>
@@ -16133,7 +16130,7 @@
         <v>7501509901018</v>
       </c>
       <c r="C131" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="D131" t="s">
         <v>97</v>
@@ -16335,7 +16332,7 @@
         <v>7501509907362</v>
       </c>
       <c r="C133" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D133" t="s">
         <v>97</v>
@@ -16436,7 +16433,7 @@
         <v>7501509907379</v>
       </c>
       <c r="C134" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="D134" t="s">
         <v>97</v>
@@ -16537,7 +16534,7 @@
         <v>7501509901049</v>
       </c>
       <c r="C135" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D135" t="s">
         <v>97</v>
@@ -16638,7 +16635,7 @@
         <v>7501509901056</v>
       </c>
       <c r="C136" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="D136" t="s">
         <v>97</v>
@@ -16840,7 +16837,7 @@
         <v>7501509900219</v>
       </c>
       <c r="C138" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="D138" t="s">
         <v>97</v>
@@ -16941,7 +16938,7 @@
         <v>7506218111666</v>
       </c>
       <c r="C139" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="D139" t="s">
         <v>97</v>
@@ -17042,7 +17039,7 @@
         <v>7501509900233</v>
       </c>
       <c r="C140" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D140" t="s">
         <v>97</v>
@@ -17143,7 +17140,7 @@
         <v>7501509900240</v>
       </c>
       <c r="C141" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D141" t="s">
         <v>97</v>
@@ -17244,7 +17241,7 @@
         <v>7501509901070</v>
       </c>
       <c r="C142" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D142" t="s">
         <v>97</v>
@@ -17345,7 +17342,7 @@
         <v>7501509901063</v>
       </c>
       <c r="C143" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="D143" t="s">
         <v>97</v>
@@ -17446,7 +17443,7 @@
         <v>7501509901087</v>
       </c>
       <c r="C144" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D144" t="s">
         <v>97</v>
@@ -17547,7 +17544,7 @@
         <v>7501509907386</v>
       </c>
       <c r="C145" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="D145" t="s">
         <v>97</v>
@@ -17648,7 +17645,7 @@
         <v>7501509907393</v>
       </c>
       <c r="C146" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="D146" t="s">
         <v>97</v>
@@ -17749,7 +17746,7 @@
         <v>7501509901094</v>
       </c>
       <c r="C147" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D147" t="s">
         <v>97</v>
@@ -17850,7 +17847,7 @@
         <v>7506218112458</v>
       </c>
       <c r="C148" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D148" t="s">
         <v>97</v>
@@ -17951,7 +17948,7 @@
         <v>7506218112229</v>
       </c>
       <c r="C149" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D149" t="s">
         <v>97</v>
@@ -18052,7 +18049,7 @@
         <v>7506218112250</v>
       </c>
       <c r="C150" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D150" t="s">
         <v>97</v>
@@ -18153,7 +18150,7 @@
         <v>7501509906693</v>
       </c>
       <c r="C151" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D151" t="s">
         <v>97</v>
@@ -18254,7 +18251,7 @@
         <v>7501509901780</v>
       </c>
       <c r="C152" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="D152" t="s">
         <v>97</v>
@@ -18355,7 +18352,7 @@
         <v>7506218110096</v>
       </c>
       <c r="C153" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D153" t="s">
         <v>97</v>
@@ -18456,7 +18453,7 @@
         <v>7506218110072</v>
       </c>
       <c r="C154" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D154" t="s">
         <v>97</v>
@@ -18557,7 +18554,7 @@
         <v>7501509901834</v>
       </c>
       <c r="C155" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="D155" t="s">
         <v>97</v>
@@ -18658,7 +18655,7 @@
         <v>7506218110102</v>
       </c>
       <c r="C156" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D156" t="s">
         <v>97</v>
@@ -18759,7 +18756,7 @@
         <v>7506218110089</v>
       </c>
       <c r="C157" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D157" t="s">
         <v>97</v>
@@ -18860,7 +18857,7 @@
         <v>7501509903234</v>
       </c>
       <c r="C158" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D158" t="s">
         <v>97</v>
@@ -18961,7 +18958,7 @@
         <v>7501509903258</v>
       </c>
       <c r="C159" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D159" t="s">
         <v>97</v>
@@ -19062,7 +19059,7 @@
         <v>7501509903241</v>
       </c>
       <c r="C160" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D160" t="s">
         <v>97</v>
@@ -19163,7 +19160,7 @@
         <v>7506218110201</v>
       </c>
       <c r="C161" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D161" t="s">
         <v>97</v>
@@ -19264,7 +19261,7 @@
         <v>7506218110256</v>
       </c>
       <c r="C162" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D162" t="s">
         <v>97</v>
@@ -19365,7 +19362,7 @@
         <v>7506218110126</v>
       </c>
       <c r="C163" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D163" t="s">
         <v>97</v>
@@ -19466,7 +19463,7 @@
         <v>7506218110119</v>
       </c>
       <c r="C164" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D164" t="s">
         <v>97</v>
@@ -19567,7 +19564,7 @@
         <v>7506218110133</v>
       </c>
       <c r="C165" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="D165" t="s">
         <v>97</v>
@@ -19668,7 +19665,7 @@
         <v>7506218110140</v>
       </c>
       <c r="C166" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D166" t="s">
         <v>97</v>

</xml_diff>

<commit_message>
Updated how data is pulled from the backend, backend server starting imports newest xlsx data
Updated the App.js fetchProducts function to check if the data imported from the backend server is different from the local storage, if it is different from the local storage, it will replace the local storage, if not, it will use the local storage. Also updated the backend server to always import the newest data from the xlsx each time the server is run.
</commit_message>
<xml_diff>
--- a/models/products.xlsx
+++ b/models/products.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\jakee\Documents\GitHub\thorsmex_digital_catalog\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{695A1911-EC5B-4B06-B7D0-651A1F7BA961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{150FE0E7-52B8-4B7E-83B6-055C59A93C28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1783,9 +1783,6 @@
     <t>Concrete Anchor 7/32" (100 Pack)</t>
   </si>
   <si>
-    <t>Concrete Anchor 7/32" &amp; Screws (20 Pack)</t>
-  </si>
-  <si>
     <t>Concrete Anchor 1/4" (20 Pack)</t>
   </si>
   <si>
@@ -1801,27 +1798,15 @@
     <t>Concrete Anchor 5/16" (100 Pack)</t>
   </si>
   <si>
-    <t>Concrete Anchor &amp; Screws 5/16" (10 Pack)</t>
-  </si>
-  <si>
-    <t>Concrete Anchor &amp; Screws 7/32" (20 Pack)</t>
-  </si>
-  <si>
     <t>Concrete Anchor 3/8" (20 Pack)</t>
   </si>
   <si>
-    <t>Concrete Anchor &amp; Screws 3/8" (6 Pack)</t>
-  </si>
-  <si>
     <t>Concrete Anchor 3/8" (100 Pack)</t>
   </si>
   <si>
     <t>Drwy Wall Anchor (20 Pack)</t>
   </si>
   <si>
-    <t>Dry Wall Anchor &amp; Nail 10x20 (100 Pack)</t>
-  </si>
-  <si>
     <t>Dry Wall Fixing Kit (40 Pack Kit)</t>
   </si>
   <si>
@@ -1837,9 +1822,6 @@
     <t>Self Drill Dry Wall Anchor (20 Pack)</t>
   </si>
   <si>
-    <t>Self Drill Dry Wall Anchor &amp; Screws (10pack)</t>
-  </si>
-  <si>
     <t>Dry wall Anchor (100 Pack)</t>
   </si>
   <si>
@@ -2135,6 +2117,24 @@
   </si>
   <si>
     <t>Floor Cord Cover Cable Black 8.2ft with Adhesive</t>
+  </si>
+  <si>
+    <t>Concrete Anchor 7/32" With Screws (20 Pack)</t>
+  </si>
+  <si>
+    <t>Concrete Anchor With Screws 7/32" (20 Pack)</t>
+  </si>
+  <si>
+    <t>Concrete Anchor With Screws 5/16" (10 Pack)</t>
+  </si>
+  <si>
+    <t>Concrete Anchor With Screws 3/8" (6 Pack)</t>
+  </si>
+  <si>
+    <t>Dry Wall Anchor With Nail 10x20 (100 Pack)</t>
+  </si>
+  <si>
+    <t>Self Drill Dry Wall Anchor With Screws (10pack)</t>
   </si>
 </sst>
 </file>
@@ -2981,8 +2981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="C122" sqref="C122"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3303,7 +3303,7 @@
         <v>7501509906228</v>
       </c>
       <c r="C4" t="s">
-        <v>395</v>
+        <v>507</v>
       </c>
       <c r="D4" t="s">
         <v>34</v>
@@ -3606,7 +3606,7 @@
         <v>7501509906235</v>
       </c>
       <c r="C7" t="s">
-        <v>402</v>
+        <v>508</v>
       </c>
       <c r="D7" t="s">
         <v>34</v>
@@ -3707,7 +3707,7 @@
         <v>7501509901889</v>
       </c>
       <c r="C8" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D8" t="s">
         <v>34</v>
@@ -3808,7 +3808,7 @@
         <v>7501509900363</v>
       </c>
       <c r="C9" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D9" t="s">
         <v>34</v>
@@ -3909,7 +3909,7 @@
         <v>7501509906242</v>
       </c>
       <c r="C10" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D10" t="s">
         <v>34</v>
@@ -4010,7 +4010,7 @@
         <v>7501509900288</v>
       </c>
       <c r="C11" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D11" t="s">
         <v>34</v>
@@ -4111,7 +4111,7 @@
         <v>7501509901896</v>
       </c>
       <c r="C12" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D12" t="s">
         <v>34</v>
@@ -4212,7 +4212,7 @@
         <v>7501509906259</v>
       </c>
       <c r="C13" t="s">
-        <v>401</v>
+        <v>509</v>
       </c>
       <c r="D13" t="s">
         <v>34</v>
@@ -4313,7 +4313,7 @@
         <v>7501509900295</v>
       </c>
       <c r="C14" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D14" t="s">
         <v>34</v>
@@ -4414,7 +4414,7 @@
         <v>7501509906266</v>
       </c>
       <c r="C15" t="s">
-        <v>404</v>
+        <v>510</v>
       </c>
       <c r="D15" t="s">
         <v>34</v>
@@ -4515,7 +4515,7 @@
         <v>7501509901902</v>
       </c>
       <c r="C16" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="D16" t="s">
         <v>34</v>
@@ -4616,7 +4616,7 @@
         <v>7501509901919</v>
       </c>
       <c r="C17" t="s">
-        <v>407</v>
+        <v>511</v>
       </c>
       <c r="D17" t="s">
         <v>34</v>
@@ -4717,7 +4717,7 @@
         <v>7501509907744</v>
       </c>
       <c r="C18" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="D18" t="s">
         <v>34</v>
@@ -4818,7 +4818,7 @@
         <v>7501509900370</v>
       </c>
       <c r="C19" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="D19" t="s">
         <v>34</v>
@@ -4919,7 +4919,7 @@
         <v>7501509901926</v>
       </c>
       <c r="C20" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="D20" t="s">
         <v>34</v>
@@ -5020,7 +5020,7 @@
         <v>7501509907737</v>
       </c>
       <c r="C21" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="D21" t="s">
         <v>34</v>
@@ -5121,7 +5121,7 @@
         <v>7501509900387</v>
       </c>
       <c r="C22" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="D22" t="s">
         <v>34</v>
@@ -5222,7 +5222,7 @@
         <v>7501509905726</v>
       </c>
       <c r="C23" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="D23" t="s">
         <v>34</v>
@@ -5323,7 +5323,7 @@
         <v>7501509905733</v>
       </c>
       <c r="C24" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="D24" t="s">
         <v>34</v>
@@ -5424,7 +5424,7 @@
         <v>7501509906556</v>
       </c>
       <c r="C25" t="s">
-        <v>413</v>
+        <v>512</v>
       </c>
       <c r="D25" t="s">
         <v>34</v>
@@ -5929,7 +5929,7 @@
         <v>7501509905955</v>
       </c>
       <c r="C30" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
       <c r="D30" t="s">
         <v>34</v>
@@ -6030,7 +6030,7 @@
         <v>7501509906013</v>
       </c>
       <c r="C31" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
       <c r="D31" t="s">
         <v>34</v>
@@ -6131,7 +6131,7 @@
         <v>7501509900899</v>
       </c>
       <c r="C32" t="s">
-        <v>416</v>
+        <v>410</v>
       </c>
       <c r="D32" t="s">
         <v>34</v>
@@ -6232,7 +6232,7 @@
         <v>7501509902060</v>
       </c>
       <c r="C33" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
       <c r="D33" t="s">
         <v>97</v>
@@ -6333,7 +6333,7 @@
         <v>7501509907751</v>
       </c>
       <c r="C34" t="s">
-        <v>418</v>
+        <v>412</v>
       </c>
       <c r="D34" t="s">
         <v>34</v>
@@ -6434,7 +6434,7 @@
         <v>7501509900905</v>
       </c>
       <c r="C35" t="s">
-        <v>416</v>
+        <v>410</v>
       </c>
       <c r="D35" t="s">
         <v>34</v>
@@ -6535,7 +6535,7 @@
         <v>7501509902077</v>
       </c>
       <c r="C36" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
       <c r="D36" t="s">
         <v>97</v>
@@ -6636,7 +6636,7 @@
         <v>7501509907768</v>
       </c>
       <c r="C37" t="s">
-        <v>418</v>
+        <v>412</v>
       </c>
       <c r="D37" t="s">
         <v>34</v>
@@ -6737,7 +6737,7 @@
         <v>7501509902084</v>
       </c>
       <c r="C38" t="s">
-        <v>419</v>
+        <v>413</v>
       </c>
       <c r="D38" t="s">
         <v>97</v>
@@ -6838,7 +6838,7 @@
         <v>7501509907775</v>
       </c>
       <c r="C39" t="s">
-        <v>420</v>
+        <v>414</v>
       </c>
       <c r="D39" t="s">
         <v>34</v>
@@ -6939,7 +6939,7 @@
         <v>7501509903999</v>
       </c>
       <c r="C40" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
       <c r="D40" t="s">
         <v>34</v>
@@ -7040,7 +7040,7 @@
         <v>7501509902091</v>
       </c>
       <c r="C41" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
       <c r="D41" t="s">
         <v>97</v>
@@ -7141,7 +7141,7 @@
         <v>7501509907782</v>
       </c>
       <c r="C42" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
       <c r="D42" t="s">
         <v>34</v>
@@ -7242,7 +7242,7 @@
         <v>7501509902107</v>
       </c>
       <c r="C43" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="D43" t="s">
         <v>97</v>
@@ -7343,7 +7343,7 @@
         <v>7501509907799</v>
       </c>
       <c r="C44" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
       <c r="D44" t="s">
         <v>34</v>
@@ -7444,7 +7444,7 @@
         <v>7501509901957</v>
       </c>
       <c r="C45" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
       <c r="D45" t="s">
         <v>34</v>
@@ -7545,7 +7545,7 @@
         <v>7501509908987</v>
       </c>
       <c r="C46" t="s">
-        <v>427</v>
+        <v>421</v>
       </c>
       <c r="D46" t="s">
         <v>34</v>
@@ -7646,7 +7646,7 @@
         <v>7501509908970</v>
       </c>
       <c r="C47" t="s">
-        <v>428</v>
+        <v>422</v>
       </c>
       <c r="D47" t="s">
         <v>34</v>
@@ -7747,7 +7747,7 @@
         <v>7501509901964</v>
       </c>
       <c r="C48" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
       <c r="D48" t="s">
         <v>97</v>
@@ -7848,7 +7848,7 @@
         <v>7506218110751</v>
       </c>
       <c r="C49" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
       <c r="D49" t="s">
         <v>97</v>
@@ -7949,7 +7949,7 @@
         <v>7501509900394</v>
       </c>
       <c r="C50" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="D50" t="s">
         <v>97</v>
@@ -8050,7 +8050,7 @@
         <v>7506218110805</v>
       </c>
       <c r="C51" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="D51" t="s">
         <v>97</v>
@@ -8151,7 +8151,7 @@
         <v>7501509901971</v>
       </c>
       <c r="C52" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="D52" t="s">
         <v>97</v>
@@ -8252,7 +8252,7 @@
         <v>7501509900400</v>
       </c>
       <c r="C53" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
       <c r="D53" t="s">
         <v>97</v>
@@ -8353,7 +8353,7 @@
         <v>7501509901988</v>
       </c>
       <c r="C54" t="s">
-        <v>452</v>
+        <v>446</v>
       </c>
       <c r="D54" t="s">
         <v>97</v>
@@ -8454,7 +8454,7 @@
         <v>7501509905313</v>
       </c>
       <c r="C55" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
       <c r="D55" t="s">
         <v>97</v>
@@ -8555,7 +8555,7 @@
         <v>7501509905771</v>
       </c>
       <c r="C56" t="s">
-        <v>452</v>
+        <v>446</v>
       </c>
       <c r="D56" t="s">
         <v>97</v>
@@ -8656,7 +8656,7 @@
         <v>7501509900417</v>
       </c>
       <c r="C57" t="s">
-        <v>454</v>
+        <v>448</v>
       </c>
       <c r="D57" t="s">
         <v>97</v>
@@ -8757,7 +8757,7 @@
         <v>7501509905641</v>
       </c>
       <c r="C58" t="s">
-        <v>454</v>
+        <v>448</v>
       </c>
       <c r="D58" t="s">
         <v>97</v>
@@ -8858,7 +8858,7 @@
         <v>7501509901995</v>
       </c>
       <c r="C59" t="s">
-        <v>455</v>
+        <v>449</v>
       </c>
       <c r="D59" t="s">
         <v>97</v>
@@ -8959,7 +8959,7 @@
         <v>7501509900844</v>
       </c>
       <c r="C60" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
       <c r="D60" t="s">
         <v>97</v>
@@ -9060,7 +9060,7 @@
         <v>7501509902008</v>
       </c>
       <c r="C61" t="s">
-        <v>457</v>
+        <v>451</v>
       </c>
       <c r="D61" t="s">
         <v>97</v>
@@ -9161,7 +9161,7 @@
         <v>7501509900127</v>
       </c>
       <c r="C62" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
       <c r="D62" t="s">
         <v>97</v>
@@ -9262,7 +9262,7 @@
         <v>7501509902022</v>
       </c>
       <c r="C63" t="s">
-        <v>455</v>
+        <v>449</v>
       </c>
       <c r="D63" t="s">
         <v>97</v>
@@ -9363,7 +9363,7 @@
         <v>7501509900851</v>
       </c>
       <c r="C64" t="s">
-        <v>459</v>
+        <v>453</v>
       </c>
       <c r="D64" t="s">
         <v>97</v>
@@ -9464,7 +9464,7 @@
         <v>7501509902039</v>
       </c>
       <c r="C65" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="D65" t="s">
         <v>97</v>
@@ -9565,7 +9565,7 @@
         <v>7501509900301</v>
       </c>
       <c r="C66" t="s">
-        <v>457</v>
+        <v>451</v>
       </c>
       <c r="D66" t="s">
         <v>97</v>
@@ -9666,7 +9666,7 @@
         <v>7501509900868</v>
       </c>
       <c r="C67" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="D67" t="s">
         <v>97</v>
@@ -9767,7 +9767,7 @@
         <v>7501509902046</v>
       </c>
       <c r="C68" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="D68" t="s">
         <v>97</v>
@@ -9868,7 +9868,7 @@
         <v>7501509900356</v>
       </c>
       <c r="C69" t="s">
-        <v>457</v>
+        <v>451</v>
       </c>
       <c r="D69" t="s">
         <v>97</v>
@@ -9969,7 +9969,7 @@
         <v>7501509900875</v>
       </c>
       <c r="C70" t="s">
-        <v>454</v>
+        <v>448</v>
       </c>
       <c r="D70" t="s">
         <v>97</v>
@@ -10070,7 +10070,7 @@
         <v>7501509902053</v>
       </c>
       <c r="C71" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="D71" t="s">
         <v>97</v>
@@ -10171,7 +10171,7 @@
         <v>7501509900882</v>
       </c>
       <c r="C72" t="s">
-        <v>454</v>
+        <v>448</v>
       </c>
       <c r="D72" t="s">
         <v>97</v>
@@ -10272,7 +10272,7 @@
         <v>7501509905795</v>
       </c>
       <c r="C73" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="D73" t="s">
         <v>97</v>
@@ -10373,7 +10373,7 @@
         <v>7501509905788</v>
       </c>
       <c r="C74" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
       <c r="D74" t="s">
         <v>97</v>
@@ -10474,7 +10474,7 @@
         <v>7501509907058</v>
       </c>
       <c r="C75" t="s">
-        <v>429</v>
+        <v>423</v>
       </c>
       <c r="D75" t="s">
         <v>97</v>
@@ -10575,7 +10575,7 @@
         <v>7506218113011</v>
       </c>
       <c r="C76" t="s">
-        <v>430</v>
+        <v>424</v>
       </c>
       <c r="D76" t="s">
         <v>34</v>
@@ -10676,7 +10676,7 @@
         <v>7506218113035</v>
       </c>
       <c r="C77" t="s">
-        <v>431</v>
+        <v>425</v>
       </c>
       <c r="D77" t="s">
         <v>34</v>
@@ -10777,7 +10777,7 @@
         <v>7501509907720</v>
       </c>
       <c r="C78" t="s">
-        <v>432</v>
+        <v>426</v>
       </c>
       <c r="D78" t="s">
         <v>97</v>
@@ -10878,7 +10878,7 @@
         <v>7501509908550</v>
       </c>
       <c r="C79" t="s">
-        <v>433</v>
+        <v>427</v>
       </c>
       <c r="D79" t="s">
         <v>97</v>
@@ -10979,7 +10979,7 @@
         <v>7501509908574</v>
       </c>
       <c r="C80" t="s">
-        <v>434</v>
+        <v>428</v>
       </c>
       <c r="D80" t="s">
         <v>97</v>
@@ -11080,7 +11080,7 @@
         <v>7501509908598</v>
       </c>
       <c r="C81" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="D81" t="s">
         <v>97</v>
@@ -11181,7 +11181,7 @@
         <v>7506218111604</v>
       </c>
       <c r="C82" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
       <c r="D82" t="s">
         <v>97</v>
@@ -11282,7 +11282,7 @@
         <v>7501509909083</v>
       </c>
       <c r="C83" t="s">
-        <v>432</v>
+        <v>426</v>
       </c>
       <c r="D83" t="s">
         <v>97</v>
@@ -11383,7 +11383,7 @@
         <v>7501509909120</v>
       </c>
       <c r="C84" t="s">
-        <v>433</v>
+        <v>427</v>
       </c>
       <c r="D84" t="s">
         <v>97</v>
@@ -11484,7 +11484,7 @@
         <v>7501509909168</v>
       </c>
       <c r="C85" t="s">
-        <v>434</v>
+        <v>428</v>
       </c>
       <c r="D85" t="s">
         <v>97</v>
@@ -11585,7 +11585,7 @@
         <v>7501509909205</v>
       </c>
       <c r="C86" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="D86" t="s">
         <v>97</v>
@@ -11686,7 +11686,7 @@
         <v>7501509907966</v>
       </c>
       <c r="C87" t="s">
-        <v>432</v>
+        <v>426</v>
       </c>
       <c r="D87" t="s">
         <v>97</v>
@@ -11787,7 +11787,7 @@
         <v>7501509908567</v>
       </c>
       <c r="C88" t="s">
-        <v>433</v>
+        <v>427</v>
       </c>
       <c r="D88" t="s">
         <v>97</v>
@@ -11888,7 +11888,7 @@
         <v>7501509908581</v>
       </c>
       <c r="C89" t="s">
-        <v>434</v>
+        <v>428</v>
       </c>
       <c r="D89" t="s">
         <v>97</v>
@@ -11989,7 +11989,7 @@
         <v>7501509908604</v>
       </c>
       <c r="C90" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="D90" t="s">
         <v>97</v>
@@ -12090,7 +12090,7 @@
         <v>7506218111611</v>
       </c>
       <c r="C91" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
       <c r="D91" t="s">
         <v>97</v>
@@ -12191,7 +12191,7 @@
         <v>7501509909809</v>
       </c>
       <c r="C92" t="s">
-        <v>432</v>
+        <v>426</v>
       </c>
       <c r="D92" t="s">
         <v>97</v>
@@ -12292,7 +12292,7 @@
         <v>7501509909816</v>
       </c>
       <c r="C93" t="s">
-        <v>433</v>
+        <v>427</v>
       </c>
       <c r="D93" t="s">
         <v>97</v>
@@ -12393,7 +12393,7 @@
         <v>7501509909823</v>
       </c>
       <c r="C94" t="s">
-        <v>434</v>
+        <v>428</v>
       </c>
       <c r="D94" t="s">
         <v>97</v>
@@ -12494,7 +12494,7 @@
         <v>7501509908246</v>
       </c>
       <c r="C95" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="D95" t="s">
         <v>97</v>
@@ -12595,7 +12595,7 @@
         <v>7501509909267</v>
       </c>
       <c r="C96" t="s">
-        <v>432</v>
+        <v>426</v>
       </c>
       <c r="D96" t="s">
         <v>97</v>
@@ -12696,7 +12696,7 @@
         <v>7501509909274</v>
       </c>
       <c r="C97" t="s">
-        <v>433</v>
+        <v>427</v>
       </c>
       <c r="D97" t="s">
         <v>97</v>
@@ -12797,7 +12797,7 @@
         <v>7501509909281</v>
       </c>
       <c r="C98" t="s">
-        <v>434</v>
+        <v>428</v>
       </c>
       <c r="D98" t="s">
         <v>97</v>
@@ -12898,7 +12898,7 @@
         <v>7501509909786</v>
       </c>
       <c r="C99" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="D99" t="s">
         <v>97</v>
@@ -12999,7 +12999,7 @@
         <v>7501509900134</v>
       </c>
       <c r="C100" t="s">
-        <v>465</v>
+        <v>459</v>
       </c>
       <c r="D100" t="s">
         <v>97</v>
@@ -13100,7 +13100,7 @@
         <v>7501509906174</v>
       </c>
       <c r="C101" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
       <c r="D101" t="s">
         <v>97</v>
@@ -13201,7 +13201,7 @@
         <v>7501509906150</v>
       </c>
       <c r="C102" t="s">
-        <v>466</v>
+        <v>460</v>
       </c>
       <c r="D102" t="s">
         <v>97</v>
@@ -13302,7 +13302,7 @@
         <v>7501509907140</v>
       </c>
       <c r="C103" t="s">
-        <v>439</v>
+        <v>433</v>
       </c>
       <c r="D103" t="s">
         <v>97</v>
@@ -13403,7 +13403,7 @@
         <v>7506218110485</v>
       </c>
       <c r="C104" t="s">
-        <v>467</v>
+        <v>461</v>
       </c>
       <c r="D104" t="s">
         <v>97</v>
@@ -13504,7 +13504,7 @@
         <v>7506218110706</v>
       </c>
       <c r="C105" t="s">
-        <v>468</v>
+        <v>462</v>
       </c>
       <c r="D105" t="s">
         <v>97</v>
@@ -13605,7 +13605,7 @@
         <v>7506218110683</v>
       </c>
       <c r="C106" t="s">
-        <v>469</v>
+        <v>463</v>
       </c>
       <c r="D106" t="s">
         <v>97</v>
@@ -13706,7 +13706,7 @@
         <v>7506218110416</v>
       </c>
       <c r="C107" t="s">
-        <v>437</v>
+        <v>431</v>
       </c>
       <c r="D107" t="s">
         <v>97</v>
@@ -13807,7 +13807,7 @@
         <v>7506218110409</v>
       </c>
       <c r="C108" t="s">
-        <v>440</v>
+        <v>434</v>
       </c>
       <c r="D108" t="s">
         <v>97</v>
@@ -13908,7 +13908,7 @@
         <v>7506218110430</v>
       </c>
       <c r="C109" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
       <c r="D109" t="s">
         <v>97</v>
@@ -14009,7 +14009,7 @@
         <v>7506218110423</v>
       </c>
       <c r="C110" t="s">
-        <v>442</v>
+        <v>436</v>
       </c>
       <c r="D110" t="s">
         <v>97</v>
@@ -14110,7 +14110,7 @@
         <v>7506218111512</v>
       </c>
       <c r="C111" t="s">
-        <v>443</v>
+        <v>437</v>
       </c>
       <c r="D111" t="s">
         <v>97</v>
@@ -14211,7 +14211,7 @@
         <v>7501509900950</v>
       </c>
       <c r="C112" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
       <c r="D112" t="s">
         <v>97</v>
@@ -14312,7 +14312,7 @@
         <v>7501509900158</v>
       </c>
       <c r="C113" t="s">
-        <v>444</v>
+        <v>438</v>
       </c>
       <c r="D113" t="s">
         <v>97</v>
@@ -14413,7 +14413,7 @@
         <v>7501509900196</v>
       </c>
       <c r="C114" t="s">
-        <v>489</v>
+        <v>483</v>
       </c>
       <c r="D114" t="s">
         <v>97</v>
@@ -14514,7 +14514,7 @@
         <v>7501509904606</v>
       </c>
       <c r="C115" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
       <c r="D115" t="s">
         <v>97</v>
@@ -14615,7 +14615,7 @@
         <v>7501509905740</v>
       </c>
       <c r="C116" t="s">
-        <v>472</v>
+        <v>466</v>
       </c>
       <c r="D116" t="s">
         <v>97</v>
@@ -14716,7 +14716,7 @@
         <v>7506218111673</v>
       </c>
       <c r="C117" t="s">
-        <v>473</v>
+        <v>467</v>
       </c>
       <c r="D117" t="s">
         <v>97</v>
@@ -14817,7 +14817,7 @@
         <v>7501509900141</v>
       </c>
       <c r="C118" t="s">
-        <v>474</v>
+        <v>468</v>
       </c>
       <c r="D118" t="s">
         <v>97</v>
@@ -14918,7 +14918,7 @@
         <v>7501509900165</v>
       </c>
       <c r="C119" t="s">
-        <v>475</v>
+        <v>469</v>
       </c>
       <c r="D119" t="s">
         <v>97</v>
@@ -15019,7 +15019,7 @@
         <v>7501509900974</v>
       </c>
       <c r="C120" t="s">
-        <v>476</v>
+        <v>470</v>
       </c>
       <c r="D120" t="s">
         <v>97</v>
@@ -15120,7 +15120,7 @@
         <v>7501509900967</v>
       </c>
       <c r="C121" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
       <c r="D121" t="s">
         <v>97</v>
@@ -15221,7 +15221,7 @@
         <v>7501509900981</v>
       </c>
       <c r="C122" t="s">
-        <v>478</v>
+        <v>472</v>
       </c>
       <c r="D122" t="s">
         <v>97</v>
@@ -15322,7 +15322,7 @@
         <v>7501509905245</v>
       </c>
       <c r="C123" t="s">
-        <v>479</v>
+        <v>473</v>
       </c>
       <c r="D123" t="s">
         <v>97</v>
@@ -15423,7 +15423,7 @@
         <v>7501509905221</v>
       </c>
       <c r="C124" t="s">
-        <v>480</v>
+        <v>474</v>
       </c>
       <c r="D124" t="s">
         <v>97</v>
@@ -15524,7 +15524,7 @@
         <v>7501509900998</v>
       </c>
       <c r="C125" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="D125" t="s">
         <v>97</v>
@@ -15625,7 +15625,7 @@
         <v>7501509901001</v>
       </c>
       <c r="C126" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
       <c r="D126" t="s">
         <v>97</v>
@@ -15726,7 +15726,7 @@
         <v>7501509900172</v>
       </c>
       <c r="C127" t="s">
-        <v>444</v>
+        <v>438</v>
       </c>
       <c r="D127" t="s">
         <v>97</v>
@@ -15827,7 +15827,7 @@
         <v>7501509900202</v>
       </c>
       <c r="C128" t="s">
-        <v>483</v>
+        <v>477</v>
       </c>
       <c r="D128" t="s">
         <v>97</v>
@@ -15928,7 +15928,7 @@
         <v>7501509900189</v>
       </c>
       <c r="C129" t="s">
-        <v>475</v>
+        <v>469</v>
       </c>
       <c r="D129" t="s">
         <v>97</v>
@@ -16029,7 +16029,7 @@
         <v>7501509901025</v>
       </c>
       <c r="C130" t="s">
-        <v>476</v>
+        <v>470</v>
       </c>
       <c r="D130" t="s">
         <v>97</v>
@@ -16130,7 +16130,7 @@
         <v>7501509901018</v>
       </c>
       <c r="C131" t="s">
-        <v>484</v>
+        <v>478</v>
       </c>
       <c r="D131" t="s">
         <v>97</v>
@@ -16231,7 +16231,7 @@
         <v>7501509901032</v>
       </c>
       <c r="C132" t="s">
-        <v>471</v>
+        <v>465</v>
       </c>
       <c r="D132" t="s">
         <v>97</v>
@@ -16332,7 +16332,7 @@
         <v>7501509907362</v>
       </c>
       <c r="C133" t="s">
-        <v>485</v>
+        <v>479</v>
       </c>
       <c r="D133" t="s">
         <v>97</v>
@@ -16433,7 +16433,7 @@
         <v>7501509907379</v>
       </c>
       <c r="C134" t="s">
-        <v>486</v>
+        <v>480</v>
       </c>
       <c r="D134" t="s">
         <v>97</v>
@@ -16534,7 +16534,7 @@
         <v>7501509901049</v>
       </c>
       <c r="C135" t="s">
-        <v>487</v>
+        <v>481</v>
       </c>
       <c r="D135" t="s">
         <v>97</v>
@@ -16635,7 +16635,7 @@
         <v>7501509901056</v>
       </c>
       <c r="C136" t="s">
-        <v>488</v>
+        <v>482</v>
       </c>
       <c r="D136" t="s">
         <v>97</v>
@@ -16736,7 +16736,7 @@
         <v>7501509900110</v>
       </c>
       <c r="C137" t="s">
-        <v>444</v>
+        <v>438</v>
       </c>
       <c r="D137" t="s">
         <v>97</v>
@@ -16837,7 +16837,7 @@
         <v>7501509900219</v>
       </c>
       <c r="C138" t="s">
-        <v>489</v>
+        <v>483</v>
       </c>
       <c r="D138" t="s">
         <v>97</v>
@@ -16938,7 +16938,7 @@
         <v>7506218111666</v>
       </c>
       <c r="C139" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="D139" t="s">
         <v>97</v>
@@ -17039,7 +17039,7 @@
         <v>7501509900233</v>
       </c>
       <c r="C140" t="s">
-        <v>475</v>
+        <v>469</v>
       </c>
       <c r="D140" t="s">
         <v>97</v>
@@ -17140,7 +17140,7 @@
         <v>7501509900240</v>
       </c>
       <c r="C141" t="s">
-        <v>475</v>
+        <v>469</v>
       </c>
       <c r="D141" t="s">
         <v>97</v>
@@ -17241,7 +17241,7 @@
         <v>7501509901070</v>
       </c>
       <c r="C142" t="s">
-        <v>491</v>
+        <v>485</v>
       </c>
       <c r="D142" t="s">
         <v>97</v>
@@ -17342,7 +17342,7 @@
         <v>7501509901063</v>
       </c>
       <c r="C143" t="s">
-        <v>492</v>
+        <v>486</v>
       </c>
       <c r="D143" t="s">
         <v>97</v>
@@ -17443,7 +17443,7 @@
         <v>7501509901087</v>
       </c>
       <c r="C144" t="s">
-        <v>493</v>
+        <v>487</v>
       </c>
       <c r="D144" t="s">
         <v>97</v>
@@ -17544,7 +17544,7 @@
         <v>7501509907386</v>
       </c>
       <c r="C145" t="s">
-        <v>494</v>
+        <v>488</v>
       </c>
       <c r="D145" t="s">
         <v>97</v>
@@ -17645,7 +17645,7 @@
         <v>7501509907393</v>
       </c>
       <c r="C146" t="s">
-        <v>495</v>
+        <v>489</v>
       </c>
       <c r="D146" t="s">
         <v>97</v>
@@ -17746,7 +17746,7 @@
         <v>7501509901094</v>
       </c>
       <c r="C147" t="s">
-        <v>496</v>
+        <v>490</v>
       </c>
       <c r="D147" t="s">
         <v>97</v>
@@ -17847,7 +17847,7 @@
         <v>7506218112458</v>
       </c>
       <c r="C148" t="s">
-        <v>497</v>
+        <v>491</v>
       </c>
       <c r="D148" t="s">
         <v>97</v>
@@ -17948,7 +17948,7 @@
         <v>7506218112229</v>
       </c>
       <c r="C149" t="s">
-        <v>498</v>
+        <v>492</v>
       </c>
       <c r="D149" t="s">
         <v>97</v>
@@ -18049,7 +18049,7 @@
         <v>7506218112250</v>
       </c>
       <c r="C150" t="s">
-        <v>499</v>
+        <v>493</v>
       </c>
       <c r="D150" t="s">
         <v>97</v>
@@ -18150,7 +18150,7 @@
         <v>7501509906693</v>
       </c>
       <c r="C151" t="s">
-        <v>500</v>
+        <v>494</v>
       </c>
       <c r="D151" t="s">
         <v>97</v>
@@ -18251,7 +18251,7 @@
         <v>7501509901780</v>
       </c>
       <c r="C152" t="s">
-        <v>501</v>
+        <v>495</v>
       </c>
       <c r="D152" t="s">
         <v>97</v>
@@ -18352,7 +18352,7 @@
         <v>7506218110096</v>
       </c>
       <c r="C153" t="s">
-        <v>502</v>
+        <v>496</v>
       </c>
       <c r="D153" t="s">
         <v>97</v>
@@ -18453,7 +18453,7 @@
         <v>7506218110072</v>
       </c>
       <c r="C154" t="s">
-        <v>503</v>
+        <v>497</v>
       </c>
       <c r="D154" t="s">
         <v>97</v>
@@ -18554,7 +18554,7 @@
         <v>7501509901834</v>
       </c>
       <c r="C155" t="s">
-        <v>501</v>
+        <v>495</v>
       </c>
       <c r="D155" t="s">
         <v>97</v>
@@ -18655,7 +18655,7 @@
         <v>7506218110102</v>
       </c>
       <c r="C156" t="s">
-        <v>502</v>
+        <v>496</v>
       </c>
       <c r="D156" t="s">
         <v>97</v>
@@ -18756,7 +18756,7 @@
         <v>7506218110089</v>
       </c>
       <c r="C157" t="s">
-        <v>503</v>
+        <v>497</v>
       </c>
       <c r="D157" t="s">
         <v>97</v>
@@ -18857,7 +18857,7 @@
         <v>7501509903234</v>
       </c>
       <c r="C158" t="s">
-        <v>510</v>
+        <v>504</v>
       </c>
       <c r="D158" t="s">
         <v>97</v>
@@ -18958,7 +18958,7 @@
         <v>7501509903258</v>
       </c>
       <c r="C159" t="s">
-        <v>511</v>
+        <v>505</v>
       </c>
       <c r="D159" t="s">
         <v>97</v>
@@ -19059,7 +19059,7 @@
         <v>7501509903241</v>
       </c>
       <c r="C160" t="s">
-        <v>512</v>
+        <v>506</v>
       </c>
       <c r="D160" t="s">
         <v>97</v>
@@ -19160,7 +19160,7 @@
         <v>7506218110201</v>
       </c>
       <c r="C161" t="s">
-        <v>509</v>
+        <v>503</v>
       </c>
       <c r="D161" t="s">
         <v>97</v>
@@ -19261,7 +19261,7 @@
         <v>7506218110256</v>
       </c>
       <c r="C162" t="s">
-        <v>508</v>
+        <v>502</v>
       </c>
       <c r="D162" t="s">
         <v>97</v>
@@ -19362,7 +19362,7 @@
         <v>7506218110126</v>
       </c>
       <c r="C163" t="s">
-        <v>507</v>
+        <v>501</v>
       </c>
       <c r="D163" t="s">
         <v>97</v>
@@ -19463,7 +19463,7 @@
         <v>7506218110119</v>
       </c>
       <c r="C164" t="s">
-        <v>506</v>
+        <v>500</v>
       </c>
       <c r="D164" t="s">
         <v>97</v>
@@ -19564,7 +19564,7 @@
         <v>7506218110133</v>
       </c>
       <c r="C165" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
       <c r="D165" t="s">
         <v>97</v>
@@ -19665,7 +19665,7 @@
         <v>7506218110140</v>
       </c>
       <c r="C166" t="s">
-        <v>504</v>
+        <v>498</v>
       </c>
       <c r="D166" t="s">
         <v>97</v>

</xml_diff>

<commit_message>
Updated error in a products title
</commit_message>
<xml_diff>
--- a/models/products.xlsx
+++ b/models/products.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\jakee\Documents\GitHub\thorsmex_digital_catalog\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{150FE0E7-52B8-4B7E-83B6-055C59A93C28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87B9551F-09A8-4C65-861F-699271764DE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1777,9 +1777,6 @@
     <t xml:space="preserve">Concrete Anchor 7/32" (20 Pack) </t>
   </si>
   <si>
-    <t>Masonry Anchor 7/32" (20 Pack)</t>
-  </si>
-  <si>
     <t>Concrete Anchor 7/32" (100 Pack)</t>
   </si>
   <si>
@@ -2135,6 +2132,9 @@
   </si>
   <si>
     <t>Self Drill Dry Wall Anchor With Screws (10pack)</t>
+  </si>
+  <si>
+    <t>Concrete Anchor 7/32" (20 Pack)</t>
   </si>
 </sst>
 </file>
@@ -2982,7 +2982,7 @@
   <dimension ref="A1:AG166"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C1:C1048576"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3101,7 +3101,7 @@
         <v>7501509901865</v>
       </c>
       <c r="C2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D2" t="s">
         <v>34</v>
@@ -3202,7 +3202,7 @@
         <v>7501509900226</v>
       </c>
       <c r="C3" t="s">
-        <v>393</v>
+        <v>512</v>
       </c>
       <c r="D3" t="s">
         <v>34</v>
@@ -3303,7 +3303,7 @@
         <v>7501509906228</v>
       </c>
       <c r="C4" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D4" t="s">
         <v>34</v>
@@ -3404,7 +3404,7 @@
         <v>7501509901872</v>
       </c>
       <c r="C5" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D5" t="s">
         <v>34</v>
@@ -3606,7 +3606,7 @@
         <v>7501509906235</v>
       </c>
       <c r="C7" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D7" t="s">
         <v>34</v>
@@ -3707,7 +3707,7 @@
         <v>7501509901889</v>
       </c>
       <c r="C8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D8" t="s">
         <v>34</v>
@@ -3808,7 +3808,7 @@
         <v>7501509900363</v>
       </c>
       <c r="C9" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D9" t="s">
         <v>34</v>
@@ -3909,7 +3909,7 @@
         <v>7501509906242</v>
       </c>
       <c r="C10" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D10" t="s">
         <v>34</v>
@@ -4010,7 +4010,7 @@
         <v>7501509900288</v>
       </c>
       <c r="C11" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D11" t="s">
         <v>34</v>
@@ -4111,7 +4111,7 @@
         <v>7501509901896</v>
       </c>
       <c r="C12" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D12" t="s">
         <v>34</v>
@@ -4212,7 +4212,7 @@
         <v>7501509906259</v>
       </c>
       <c r="C13" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D13" t="s">
         <v>34</v>
@@ -4313,7 +4313,7 @@
         <v>7501509900295</v>
       </c>
       <c r="C14" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D14" t="s">
         <v>34</v>
@@ -4414,7 +4414,7 @@
         <v>7501509906266</v>
       </c>
       <c r="C15" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D15" t="s">
         <v>34</v>
@@ -4515,7 +4515,7 @@
         <v>7501509901902</v>
       </c>
       <c r="C16" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D16" t="s">
         <v>34</v>
@@ -4616,7 +4616,7 @@
         <v>7501509901919</v>
       </c>
       <c r="C17" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D17" t="s">
         <v>34</v>
@@ -4717,7 +4717,7 @@
         <v>7501509907744</v>
       </c>
       <c r="C18" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D18" t="s">
         <v>34</v>
@@ -4818,7 +4818,7 @@
         <v>7501509900370</v>
       </c>
       <c r="C19" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D19" t="s">
         <v>34</v>
@@ -4919,7 +4919,7 @@
         <v>7501509901926</v>
       </c>
       <c r="C20" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D20" t="s">
         <v>34</v>
@@ -5020,7 +5020,7 @@
         <v>7501509907737</v>
       </c>
       <c r="C21" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D21" t="s">
         <v>34</v>
@@ -5121,7 +5121,7 @@
         <v>7501509900387</v>
       </c>
       <c r="C22" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D22" t="s">
         <v>34</v>
@@ -5222,7 +5222,7 @@
         <v>7501509905726</v>
       </c>
       <c r="C23" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D23" t="s">
         <v>34</v>
@@ -5323,7 +5323,7 @@
         <v>7501509905733</v>
       </c>
       <c r="C24" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D24" t="s">
         <v>34</v>
@@ -5424,7 +5424,7 @@
         <v>7501509906556</v>
       </c>
       <c r="C25" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D25" t="s">
         <v>34</v>
@@ -5929,7 +5929,7 @@
         <v>7501509905955</v>
       </c>
       <c r="C30" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D30" t="s">
         <v>34</v>
@@ -6030,7 +6030,7 @@
         <v>7501509906013</v>
       </c>
       <c r="C31" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D31" t="s">
         <v>34</v>
@@ -6131,7 +6131,7 @@
         <v>7501509900899</v>
       </c>
       <c r="C32" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D32" t="s">
         <v>34</v>
@@ -6232,7 +6232,7 @@
         <v>7501509902060</v>
       </c>
       <c r="C33" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D33" t="s">
         <v>97</v>
@@ -6333,7 +6333,7 @@
         <v>7501509907751</v>
       </c>
       <c r="C34" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D34" t="s">
         <v>34</v>
@@ -6434,7 +6434,7 @@
         <v>7501509900905</v>
       </c>
       <c r="C35" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D35" t="s">
         <v>34</v>
@@ -6535,7 +6535,7 @@
         <v>7501509902077</v>
       </c>
       <c r="C36" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D36" t="s">
         <v>97</v>
@@ -6636,7 +6636,7 @@
         <v>7501509907768</v>
       </c>
       <c r="C37" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D37" t="s">
         <v>34</v>
@@ -6737,7 +6737,7 @@
         <v>7501509902084</v>
       </c>
       <c r="C38" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D38" t="s">
         <v>97</v>
@@ -6838,7 +6838,7 @@
         <v>7501509907775</v>
       </c>
       <c r="C39" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D39" t="s">
         <v>34</v>
@@ -6939,7 +6939,7 @@
         <v>7501509903999</v>
       </c>
       <c r="C40" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D40" t="s">
         <v>34</v>
@@ -7040,7 +7040,7 @@
         <v>7501509902091</v>
       </c>
       <c r="C41" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D41" t="s">
         <v>97</v>
@@ -7141,7 +7141,7 @@
         <v>7501509907782</v>
       </c>
       <c r="C42" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D42" t="s">
         <v>34</v>
@@ -7242,7 +7242,7 @@
         <v>7501509902107</v>
       </c>
       <c r="C43" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D43" t="s">
         <v>97</v>
@@ -7343,7 +7343,7 @@
         <v>7501509907799</v>
       </c>
       <c r="C44" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D44" t="s">
         <v>34</v>
@@ -7444,7 +7444,7 @@
         <v>7501509901957</v>
       </c>
       <c r="C45" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D45" t="s">
         <v>34</v>
@@ -7545,7 +7545,7 @@
         <v>7501509908987</v>
       </c>
       <c r="C46" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D46" t="s">
         <v>34</v>
@@ -7646,7 +7646,7 @@
         <v>7501509908970</v>
       </c>
       <c r="C47" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D47" t="s">
         <v>34</v>
@@ -7747,7 +7747,7 @@
         <v>7501509901964</v>
       </c>
       <c r="C48" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D48" t="s">
         <v>97</v>
@@ -7848,7 +7848,7 @@
         <v>7506218110751</v>
       </c>
       <c r="C49" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D49" t="s">
         <v>97</v>
@@ -7949,7 +7949,7 @@
         <v>7501509900394</v>
       </c>
       <c r="C50" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D50" t="s">
         <v>97</v>
@@ -8050,7 +8050,7 @@
         <v>7506218110805</v>
       </c>
       <c r="C51" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D51" t="s">
         <v>97</v>
@@ -8151,7 +8151,7 @@
         <v>7501509901971</v>
       </c>
       <c r="C52" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D52" t="s">
         <v>97</v>
@@ -8252,7 +8252,7 @@
         <v>7501509900400</v>
       </c>
       <c r="C53" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D53" t="s">
         <v>97</v>
@@ -8353,7 +8353,7 @@
         <v>7501509901988</v>
       </c>
       <c r="C54" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D54" t="s">
         <v>97</v>
@@ -8454,7 +8454,7 @@
         <v>7501509905313</v>
       </c>
       <c r="C55" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D55" t="s">
         <v>97</v>
@@ -8555,7 +8555,7 @@
         <v>7501509905771</v>
       </c>
       <c r="C56" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D56" t="s">
         <v>97</v>
@@ -8656,7 +8656,7 @@
         <v>7501509900417</v>
       </c>
       <c r="C57" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D57" t="s">
         <v>97</v>
@@ -8757,7 +8757,7 @@
         <v>7501509905641</v>
       </c>
       <c r="C58" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D58" t="s">
         <v>97</v>
@@ -8858,7 +8858,7 @@
         <v>7501509901995</v>
       </c>
       <c r="C59" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D59" t="s">
         <v>97</v>
@@ -8959,7 +8959,7 @@
         <v>7501509900844</v>
       </c>
       <c r="C60" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D60" t="s">
         <v>97</v>
@@ -9060,7 +9060,7 @@
         <v>7501509902008</v>
       </c>
       <c r="C61" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D61" t="s">
         <v>97</v>
@@ -9161,7 +9161,7 @@
         <v>7501509900127</v>
       </c>
       <c r="C62" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D62" t="s">
         <v>97</v>
@@ -9262,7 +9262,7 @@
         <v>7501509902022</v>
       </c>
       <c r="C63" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D63" t="s">
         <v>97</v>
@@ -9363,7 +9363,7 @@
         <v>7501509900851</v>
       </c>
       <c r="C64" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D64" t="s">
         <v>97</v>
@@ -9464,7 +9464,7 @@
         <v>7501509902039</v>
       </c>
       <c r="C65" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D65" t="s">
         <v>97</v>
@@ -9565,7 +9565,7 @@
         <v>7501509900301</v>
       </c>
       <c r="C66" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D66" t="s">
         <v>97</v>
@@ -9666,7 +9666,7 @@
         <v>7501509900868</v>
       </c>
       <c r="C67" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D67" t="s">
         <v>97</v>
@@ -9767,7 +9767,7 @@
         <v>7501509902046</v>
       </c>
       <c r="C68" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D68" t="s">
         <v>97</v>
@@ -9868,7 +9868,7 @@
         <v>7501509900356</v>
       </c>
       <c r="C69" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D69" t="s">
         <v>97</v>
@@ -9969,7 +9969,7 @@
         <v>7501509900875</v>
       </c>
       <c r="C70" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D70" t="s">
         <v>97</v>
@@ -10070,7 +10070,7 @@
         <v>7501509902053</v>
       </c>
       <c r="C71" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D71" t="s">
         <v>97</v>
@@ -10171,7 +10171,7 @@
         <v>7501509900882</v>
       </c>
       <c r="C72" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D72" t="s">
         <v>97</v>
@@ -10272,7 +10272,7 @@
         <v>7501509905795</v>
       </c>
       <c r="C73" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D73" t="s">
         <v>97</v>
@@ -10373,7 +10373,7 @@
         <v>7501509905788</v>
       </c>
       <c r="C74" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D74" t="s">
         <v>97</v>
@@ -10474,7 +10474,7 @@
         <v>7501509907058</v>
       </c>
       <c r="C75" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D75" t="s">
         <v>97</v>
@@ -10575,7 +10575,7 @@
         <v>7506218113011</v>
       </c>
       <c r="C76" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D76" t="s">
         <v>34</v>
@@ -10676,7 +10676,7 @@
         <v>7506218113035</v>
       </c>
       <c r="C77" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D77" t="s">
         <v>34</v>
@@ -10777,7 +10777,7 @@
         <v>7501509907720</v>
       </c>
       <c r="C78" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D78" t="s">
         <v>97</v>
@@ -10878,7 +10878,7 @@
         <v>7501509908550</v>
       </c>
       <c r="C79" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D79" t="s">
         <v>97</v>
@@ -10979,7 +10979,7 @@
         <v>7501509908574</v>
       </c>
       <c r="C80" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D80" t="s">
         <v>97</v>
@@ -11080,7 +11080,7 @@
         <v>7501509908598</v>
       </c>
       <c r="C81" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D81" t="s">
         <v>97</v>
@@ -11181,7 +11181,7 @@
         <v>7506218111604</v>
       </c>
       <c r="C82" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D82" t="s">
         <v>97</v>
@@ -11282,7 +11282,7 @@
         <v>7501509909083</v>
       </c>
       <c r="C83" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D83" t="s">
         <v>97</v>
@@ -11383,7 +11383,7 @@
         <v>7501509909120</v>
       </c>
       <c r="C84" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D84" t="s">
         <v>97</v>
@@ -11484,7 +11484,7 @@
         <v>7501509909168</v>
       </c>
       <c r="C85" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D85" t="s">
         <v>97</v>
@@ -11585,7 +11585,7 @@
         <v>7501509909205</v>
       </c>
       <c r="C86" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D86" t="s">
         <v>97</v>
@@ -11686,7 +11686,7 @@
         <v>7501509907966</v>
       </c>
       <c r="C87" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D87" t="s">
         <v>97</v>
@@ -11787,7 +11787,7 @@
         <v>7501509908567</v>
       </c>
       <c r="C88" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D88" t="s">
         <v>97</v>
@@ -11888,7 +11888,7 @@
         <v>7501509908581</v>
       </c>
       <c r="C89" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D89" t="s">
         <v>97</v>
@@ -11989,7 +11989,7 @@
         <v>7501509908604</v>
       </c>
       <c r="C90" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D90" t="s">
         <v>97</v>
@@ -12090,7 +12090,7 @@
         <v>7506218111611</v>
       </c>
       <c r="C91" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D91" t="s">
         <v>97</v>
@@ -12191,7 +12191,7 @@
         <v>7501509909809</v>
       </c>
       <c r="C92" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D92" t="s">
         <v>97</v>
@@ -12292,7 +12292,7 @@
         <v>7501509909816</v>
       </c>
       <c r="C93" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D93" t="s">
         <v>97</v>
@@ -12393,7 +12393,7 @@
         <v>7501509909823</v>
       </c>
       <c r="C94" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D94" t="s">
         <v>97</v>
@@ -12494,7 +12494,7 @@
         <v>7501509908246</v>
       </c>
       <c r="C95" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D95" t="s">
         <v>97</v>
@@ -12595,7 +12595,7 @@
         <v>7501509909267</v>
       </c>
       <c r="C96" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D96" t="s">
         <v>97</v>
@@ -12696,7 +12696,7 @@
         <v>7501509909274</v>
       </c>
       <c r="C97" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D97" t="s">
         <v>97</v>
@@ -12797,7 +12797,7 @@
         <v>7501509909281</v>
       </c>
       <c r="C98" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D98" t="s">
         <v>97</v>
@@ -12898,7 +12898,7 @@
         <v>7501509909786</v>
       </c>
       <c r="C99" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D99" t="s">
         <v>97</v>
@@ -12999,7 +12999,7 @@
         <v>7501509900134</v>
       </c>
       <c r="C100" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="D100" t="s">
         <v>97</v>
@@ -13100,7 +13100,7 @@
         <v>7501509906174</v>
       </c>
       <c r="C101" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D101" t="s">
         <v>97</v>
@@ -13201,7 +13201,7 @@
         <v>7501509906150</v>
       </c>
       <c r="C102" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D102" t="s">
         <v>97</v>
@@ -13302,7 +13302,7 @@
         <v>7501509907140</v>
       </c>
       <c r="C103" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D103" t="s">
         <v>97</v>
@@ -13403,7 +13403,7 @@
         <v>7506218110485</v>
       </c>
       <c r="C104" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D104" t="s">
         <v>97</v>
@@ -13504,7 +13504,7 @@
         <v>7506218110706</v>
       </c>
       <c r="C105" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="D105" t="s">
         <v>97</v>
@@ -13605,7 +13605,7 @@
         <v>7506218110683</v>
       </c>
       <c r="C106" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D106" t="s">
         <v>97</v>
@@ -13706,7 +13706,7 @@
         <v>7506218110416</v>
       </c>
       <c r="C107" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D107" t="s">
         <v>97</v>
@@ -13807,7 +13807,7 @@
         <v>7506218110409</v>
       </c>
       <c r="C108" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D108" t="s">
         <v>97</v>
@@ -13908,7 +13908,7 @@
         <v>7506218110430</v>
       </c>
       <c r="C109" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D109" t="s">
         <v>97</v>
@@ -14009,7 +14009,7 @@
         <v>7506218110423</v>
       </c>
       <c r="C110" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D110" t="s">
         <v>97</v>
@@ -14110,7 +14110,7 @@
         <v>7506218111512</v>
       </c>
       <c r="C111" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D111" t="s">
         <v>97</v>
@@ -14211,7 +14211,7 @@
         <v>7501509900950</v>
       </c>
       <c r="C112" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D112" t="s">
         <v>97</v>
@@ -14312,7 +14312,7 @@
         <v>7501509900158</v>
       </c>
       <c r="C113" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D113" t="s">
         <v>97</v>
@@ -14413,7 +14413,7 @@
         <v>7501509900196</v>
       </c>
       <c r="C114" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="D114" t="s">
         <v>97</v>
@@ -14514,7 +14514,7 @@
         <v>7501509904606</v>
       </c>
       <c r="C115" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="D115" t="s">
         <v>97</v>
@@ -14615,7 +14615,7 @@
         <v>7501509905740</v>
       </c>
       <c r="C116" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D116" t="s">
         <v>97</v>
@@ -14716,7 +14716,7 @@
         <v>7506218111673</v>
       </c>
       <c r="C117" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D117" t="s">
         <v>97</v>
@@ -14817,7 +14817,7 @@
         <v>7501509900141</v>
       </c>
       <c r="C118" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D118" t="s">
         <v>97</v>
@@ -14918,7 +14918,7 @@
         <v>7501509900165</v>
       </c>
       <c r="C119" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D119" t="s">
         <v>97</v>
@@ -15019,7 +15019,7 @@
         <v>7501509900974</v>
       </c>
       <c r="C120" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="D120" t="s">
         <v>97</v>
@@ -15120,7 +15120,7 @@
         <v>7501509900967</v>
       </c>
       <c r="C121" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="D121" t="s">
         <v>97</v>
@@ -15221,7 +15221,7 @@
         <v>7501509900981</v>
       </c>
       <c r="C122" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="D122" t="s">
         <v>97</v>
@@ -15322,7 +15322,7 @@
         <v>7501509905245</v>
       </c>
       <c r="C123" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D123" t="s">
         <v>97</v>
@@ -15423,7 +15423,7 @@
         <v>7501509905221</v>
       </c>
       <c r="C124" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D124" t="s">
         <v>97</v>
@@ -15524,7 +15524,7 @@
         <v>7501509900998</v>
       </c>
       <c r="C125" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D125" t="s">
         <v>97</v>
@@ -15625,7 +15625,7 @@
         <v>7501509901001</v>
       </c>
       <c r="C126" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D126" t="s">
         <v>97</v>
@@ -15726,7 +15726,7 @@
         <v>7501509900172</v>
       </c>
       <c r="C127" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D127" t="s">
         <v>97</v>
@@ -15827,7 +15827,7 @@
         <v>7501509900202</v>
       </c>
       <c r="C128" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D128" t="s">
         <v>97</v>
@@ -15928,7 +15928,7 @@
         <v>7501509900189</v>
       </c>
       <c r="C129" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D129" t="s">
         <v>97</v>
@@ -16029,7 +16029,7 @@
         <v>7501509901025</v>
       </c>
       <c r="C130" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="D130" t="s">
         <v>97</v>
@@ -16130,7 +16130,7 @@
         <v>7501509901018</v>
       </c>
       <c r="C131" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D131" t="s">
         <v>97</v>
@@ -16231,7 +16231,7 @@
         <v>7501509901032</v>
       </c>
       <c r="C132" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D132" t="s">
         <v>97</v>
@@ -16332,7 +16332,7 @@
         <v>7501509907362</v>
       </c>
       <c r="C133" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D133" t="s">
         <v>97</v>
@@ -16433,7 +16433,7 @@
         <v>7501509907379</v>
       </c>
       <c r="C134" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D134" t="s">
         <v>97</v>
@@ -16534,7 +16534,7 @@
         <v>7501509901049</v>
       </c>
       <c r="C135" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D135" t="s">
         <v>97</v>
@@ -16635,7 +16635,7 @@
         <v>7501509901056</v>
       </c>
       <c r="C136" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="D136" t="s">
         <v>97</v>
@@ -16736,7 +16736,7 @@
         <v>7501509900110</v>
       </c>
       <c r="C137" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D137" t="s">
         <v>97</v>
@@ -16837,7 +16837,7 @@
         <v>7501509900219</v>
       </c>
       <c r="C138" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="D138" t="s">
         <v>97</v>
@@ -16938,7 +16938,7 @@
         <v>7506218111666</v>
       </c>
       <c r="C139" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D139" t="s">
         <v>97</v>
@@ -17039,7 +17039,7 @@
         <v>7501509900233</v>
       </c>
       <c r="C140" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D140" t="s">
         <v>97</v>
@@ -17140,7 +17140,7 @@
         <v>7501509900240</v>
       </c>
       <c r="C141" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D141" t="s">
         <v>97</v>
@@ -17241,7 +17241,7 @@
         <v>7501509901070</v>
       </c>
       <c r="C142" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="D142" t="s">
         <v>97</v>
@@ -17342,7 +17342,7 @@
         <v>7501509901063</v>
       </c>
       <c r="C143" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D143" t="s">
         <v>97</v>
@@ -17443,7 +17443,7 @@
         <v>7501509901087</v>
       </c>
       <c r="C144" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="D144" t="s">
         <v>97</v>
@@ -17544,7 +17544,7 @@
         <v>7501509907386</v>
       </c>
       <c r="C145" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D145" t="s">
         <v>97</v>
@@ -17645,7 +17645,7 @@
         <v>7501509907393</v>
       </c>
       <c r="C146" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="D146" t="s">
         <v>97</v>
@@ -17746,7 +17746,7 @@
         <v>7501509901094</v>
       </c>
       <c r="C147" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="D147" t="s">
         <v>97</v>
@@ -17847,7 +17847,7 @@
         <v>7506218112458</v>
       </c>
       <c r="C148" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="D148" t="s">
         <v>97</v>
@@ -17948,7 +17948,7 @@
         <v>7506218112229</v>
       </c>
       <c r="C149" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D149" t="s">
         <v>97</v>
@@ -18049,7 +18049,7 @@
         <v>7506218112250</v>
       </c>
       <c r="C150" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="D150" t="s">
         <v>97</v>
@@ -18150,7 +18150,7 @@
         <v>7501509906693</v>
       </c>
       <c r="C151" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D151" t="s">
         <v>97</v>
@@ -18251,7 +18251,7 @@
         <v>7501509901780</v>
       </c>
       <c r="C152" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="D152" t="s">
         <v>97</v>
@@ -18352,7 +18352,7 @@
         <v>7506218110096</v>
       </c>
       <c r="C153" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="D153" t="s">
         <v>97</v>
@@ -18453,7 +18453,7 @@
         <v>7506218110072</v>
       </c>
       <c r="C154" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D154" t="s">
         <v>97</v>
@@ -18554,7 +18554,7 @@
         <v>7501509901834</v>
       </c>
       <c r="C155" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="D155" t="s">
         <v>97</v>
@@ -18655,7 +18655,7 @@
         <v>7506218110102</v>
       </c>
       <c r="C156" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="D156" t="s">
         <v>97</v>
@@ -18756,7 +18756,7 @@
         <v>7506218110089</v>
       </c>
       <c r="C157" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D157" t="s">
         <v>97</v>
@@ -18857,7 +18857,7 @@
         <v>7501509903234</v>
       </c>
       <c r="C158" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D158" t="s">
         <v>97</v>
@@ -18958,7 +18958,7 @@
         <v>7501509903258</v>
       </c>
       <c r="C159" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D159" t="s">
         <v>97</v>
@@ -19059,7 +19059,7 @@
         <v>7501509903241</v>
       </c>
       <c r="C160" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="D160" t="s">
         <v>97</v>
@@ -19160,7 +19160,7 @@
         <v>7506218110201</v>
       </c>
       <c r="C161" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D161" t="s">
         <v>97</v>
@@ -19261,7 +19261,7 @@
         <v>7506218110256</v>
       </c>
       <c r="C162" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="D162" t="s">
         <v>97</v>
@@ -19362,7 +19362,7 @@
         <v>7506218110126</v>
       </c>
       <c r="C163" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D163" t="s">
         <v>97</v>
@@ -19463,7 +19463,7 @@
         <v>7506218110119</v>
       </c>
       <c r="C164" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D164" t="s">
         <v>97</v>
@@ -19564,7 +19564,7 @@
         <v>7506218110133</v>
       </c>
       <c r="C165" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D165" t="s">
         <v>97</v>
@@ -19665,7 +19665,7 @@
         <v>7506218110140</v>
       </c>
       <c r="C166" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D166" t="s">
         <v>97</v>

</xml_diff>